<commit_message>
fixed broken upload issue.
</commit_message>
<xml_diff>
--- a/host/static/Users.xlsx
+++ b/host/static/Users.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -402,7 +402,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -447,7 +447,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -481,10 +481,55 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>1111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>joe</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>42132</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Graham Gibson</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Queen's University</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>1111111</t>
         </is>

</xml_diff>